<commit_message>
temp:临时节点标记 星期二 晚上 8:51:47 七月 19日 2022 创建了 src/utils/get_filelist_detail.js 修改了 electron/ipcMain.js 修改了 package.json 修改了 src/pages/MainPage/components/insert_expect/index.js 修改了 src/pages/MainPage/elements/upload_dragger/index.js 修改了 src/pages/MainPage/index.js 修改了 "statics/\345\244\252\346\230\216\346\210\220\346\234\254(\345\217\221\347\245\250\346\225\260\346\215\256).xlsx"
</commit_message>
<xml_diff>
--- a/statics/太明成本(发票数据).xlsx
+++ b/statics/太明成本(发票数据).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shicheng.yu/Desktop/独立开发项目/客户端项目/excel-helper-client/server/statics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shicheng.yu/Desktop/独立开发项目/在线图片签名项目/客户端项目/private-computed-helper/statics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D08F004-FFCB-5346-BD3A-DF5CD3047D13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED84082F-04EC-3A4E-8A1E-9C381B8EC5E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t>入库产品生产分配明细表</t>
   </si>
@@ -50,6 +50,10 @@
   </si>
   <si>
     <t>合计</t>
+  </si>
+  <si>
+    <t>填写入库产品的销售数</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -486,7 +490,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -565,45 +569,75 @@
     <row r="6" spans="1:7" ht="24" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="21" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="21" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>

</xml_diff>